<commit_message>
add page 404 and change _nav.ts
</commit_message>
<xml_diff>
--- a/API/Resources/Template/Article/ArticleListTemplate.xlsx
+++ b/API/Resources/Template/Article/ArticleListTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HIEU\hoc\Dropzone\API\Resources\Template\Article\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HIEU\hoc\DropzoneUpdate\API\Resources\Template\Article\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Status</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>&amp;=result.Article_Cate_ID</t>
-  </si>
-  <si>
-    <t>&amp;=result.Status</t>
   </si>
 </sst>
 </file>
@@ -436,7 +433,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +469,7 @@
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -482,9 +479,7 @@
       <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
         <v>7</v>
       </c>

</xml_diff>